<commit_message>
updated comparison analysis with new INCa funding agency
</commit_message>
<xml_diff>
--- a/output/comparison_statistics.xlsx
+++ b/output/comparison_statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nj995/dropbox/projects/2018_helios/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F9E65506-EE91-064F-8377-F3811E4F7BF1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F93DC832-99AA-9340-A6D3-F28E596A4591}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,23 +21,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
+  <si>
+    <t>INCa</t>
+  </si>
+  <si>
+    <t>INSERM</t>
+  </si>
+  <si>
+    <t>INCa - ORCID Confirmed</t>
+  </si>
+  <si>
+    <t>INSERM - ORCID Confirmed</t>
+  </si>
   <si>
     <t>Cancer Research UK</t>
   </si>
   <si>
-    <t>INSERM</t>
-  </si>
-  <si>
-    <t>INSERM - ORCID Confirmed</t>
-  </si>
-  <si>
-    <t>INCa</t>
-  </si>
-  <si>
-    <t>INCa - ORCID Confirmed</t>
-  </si>
-  <si>
     <t>National Cancer Institute</t>
   </si>
   <si>
@@ -47,18 +47,18 @@
     <t>Wellcome Trust</t>
   </si>
   <si>
+    <t>French National Cancer Institute</t>
+  </si>
+  <si>
     <t>French Institute of Health and Medical Research</t>
   </si>
   <si>
+    <t>French National Cancer Institute - ORCID Confirmed</t>
+  </si>
+  <si>
     <t>French Institute of Health and Medical Research - ORCID Confirmed</t>
   </si>
   <si>
-    <t>French National Cancer Institute</t>
-  </si>
-  <si>
-    <t>French National Cancer Institute - ORCID Confirmed</t>
-  </si>
-  <si>
     <t>Number of Grants Funded between 2007 and 2012</t>
   </si>
   <si>
@@ -281,6 +281,12 @@
     <t>post_citations_med</t>
   </si>
   <si>
+    <t>Ministère des Affaires sociales et de la Santé</t>
+  </si>
+  <si>
+    <t>Ministère des Affaires sociales et de la Santé - ORCID Confirmed</t>
+  </si>
+  <si>
     <t>Cancer</t>
   </si>
   <si>
@@ -293,10 +299,19 @@
     <t>Genetics</t>
   </si>
   <si>
+    <t>Clinical Trials and Supportive Activities</t>
+  </si>
+  <si>
     <t>Biotechnology</t>
   </si>
   <si>
     <t>Prevention</t>
+  </si>
+  <si>
+    <t>Patient Safety</t>
+  </si>
+  <si>
+    <t>Hematology</t>
   </si>
   <si>
     <t>Digestive Diseases</t>
@@ -311,9 +326,16 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -369,7 +391,6 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -513,42 +534,43 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -856,10 +878,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -867,67 +889,79 @@
     <col min="1" max="1" width="48.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="6" hidden="1" customWidth="1" outlineLevel="1"/>
     <col min="3" max="3" width="16.6640625" style="6" customWidth="1" collapsed="1"/>
-    <col min="4" max="10" width="16.6640625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="6" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="6"/>
+    <col min="4" max="12" width="16.6640625" style="6" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="49" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="65" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7"/>
       <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="24" t="s">
+      <c r="G2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="K2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:10" collapsed="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -935,39 +969,47 @@
         <v>13</v>
       </c>
       <c r="C3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>730</v>
       </c>
       <c r="D3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>114</v>
       </c>
       <c r="E3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>406</v>
+      </c>
+      <c r="F3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>132</v>
       </c>
-      <c r="F3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>35</v>
       </c>
-      <c r="G3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>64</v>
+      </c>
+      <c r="I3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>2225</v>
       </c>
-      <c r="H3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>12468</v>
       </c>
-      <c r="I3" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K3" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1064</v>
       </c>
-      <c r="J3" s="11">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B3, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L3" s="11">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B3, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>261</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>14</v>
       </c>
@@ -975,119 +1017,143 @@
         <v>15</v>
       </c>
       <c r="C4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>669</v>
       </c>
       <c r="D4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>122</v>
       </c>
       <c r="E4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>333</v>
+      </c>
+      <c r="F4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>95</v>
       </c>
-      <c r="F4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>34</v>
       </c>
-      <c r="G4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>50</v>
+      </c>
+      <c r="I4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1370</v>
       </c>
-      <c r="H4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>8450</v>
       </c>
-      <c r="I4" s="10">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K4" s="10">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1944</v>
       </c>
-      <c r="J4" s="11">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B4, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L4" s="11">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B4, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>328</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>557125.4734876774</v>
       </c>
-      <c r="D5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+      <c r="D5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>234241.09649122809</v>
       </c>
-      <c r="E5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+      <c r="E5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>442562.60098522168</v>
+      </c>
+      <c r="F5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>464458.65151515149</v>
       </c>
-      <c r="F5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>232874.28571428571</v>
       </c>
-      <c r="G5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>420509.171875</v>
+      </c>
+      <c r="I5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1856361.57394931</v>
       </c>
-      <c r="I5" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K5" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>609689.00565504236</v>
       </c>
-      <c r="J5" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B5, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L5" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B5, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>797713.74712643679</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>417676</v>
       </c>
-      <c r="D6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+      <c r="D6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>201539.5</v>
       </c>
-      <c r="E6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+      <c r="E6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>390888.5</v>
+      </c>
+      <c r="F6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>471555</v>
       </c>
-      <c r="F6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>235320</v>
       </c>
-      <c r="G6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>363145</v>
+      </c>
+      <c r="I6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="J6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>732061</v>
       </c>
-      <c r="I6" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K6" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>433722</v>
       </c>
-      <c r="J6" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B6, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L6" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B6, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>325304</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1095,39 +1161,47 @@
         <v>21</v>
       </c>
       <c r="C7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>2.7330829613667742</v>
       </c>
       <c r="D7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>2.1501515335192152</v>
       </c>
       <c r="E7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>3.194426074633903</v>
+      </c>
+      <c r="F7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>2.6584059775840601</v>
       </c>
-      <c r="F7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>2.0821135029354201</v>
       </c>
-      <c r="G7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>3.114340753424655</v>
+      </c>
+      <c r="I7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>3.372390949669076</v>
       </c>
-      <c r="H7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>4.2549639405647506</v>
       </c>
-      <c r="I7" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K7" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>2.8267044860399211</v>
       </c>
-      <c r="J7" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B7, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L7" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B7, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>3.2201228153046779</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>22</v>
       </c>
@@ -1135,39 +1209,47 @@
         <v>23</v>
       </c>
       <c r="C8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>3</v>
       </c>
       <c r="D8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>2</v>
       </c>
       <c r="E8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>3.0027397260273969</v>
+      </c>
+      <c r="F8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>3</v>
       </c>
-      <c r="F8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>1.9972602739726031</v>
       </c>
-      <c r="G8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>3.0027397260273969</v>
+      </c>
+      <c r="I8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>3</v>
       </c>
-      <c r="H8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>3.9589041095890409</v>
       </c>
-      <c r="I8" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K8" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>3</v>
       </c>
-      <c r="J8" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B8, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L8" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B8, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>3.0849315068493151</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>24</v>
       </c>
@@ -1175,39 +1257,47 @@
         <v>25</v>
       </c>
       <c r="C9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>1.383861236802413</v>
       </c>
       <c r="D9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>1.1140350877192979</v>
       </c>
       <c r="E9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>1.157635467980296</v>
+      </c>
+      <c r="F9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>1.492424242424242</v>
       </c>
-      <c r="F9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>1.0857142857142861</v>
       </c>
-      <c r="G9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>1.234375</v>
+      </c>
+      <c r="I9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1.016644174538911</v>
       </c>
-      <c r="H9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1.104041853008185</v>
       </c>
-      <c r="I9" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K9" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>2.6992481203007519</v>
       </c>
-      <c r="J9" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B9, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L9" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B9, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1.57088122605364</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>26</v>
       </c>
@@ -1215,39 +1305,47 @@
         <v>27</v>
       </c>
       <c r="C10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="D10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="E10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="F10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="G10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="H10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
       <c r="I10" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>1</v>
+      </c>
+      <c r="J10" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+        <v>1</v>
+      </c>
+      <c r="K10" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>2</v>
       </c>
-      <c r="J10" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B10, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L10" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B10, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>28</v>
       </c>
@@ -1255,39 +1353,47 @@
         <v>29</v>
       </c>
       <c r="C11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="D11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="E11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="F11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="G11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="H11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
       <c r="I11" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
-      <c r="J11" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B11, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J11" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>Cancer</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
+        <v>Cancer</v>
+      </c>
+      <c r="L11" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B11, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
+        <v>Cancer</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>30</v>
       </c>
@@ -1295,39 +1401,47 @@
         <v>31</v>
       </c>
       <c r="C12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
       <c r="D12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
       <c r="E12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Research</v>
+      </c>
+      <c r="F12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
-      <c r="F12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>Genetics</v>
       </c>
-      <c r="G12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v>Clinical Research</v>
       </c>
-      <c r="H12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="I12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>Clinical Research</v>
       </c>
-      <c r="I12" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Research</v>
+      </c>
+      <c r="K12" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
-      <c r="J12" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B12, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L12" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B12, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>Genetics</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>32</v>
       </c>
@@ -1335,39 +1449,47 @@
         <v>33</v>
       </c>
       <c r="C13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>Genetics</v>
       </c>
       <c r="D13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Research</v>
+      </c>
+      <c r="E13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>Rare Diseases</v>
+      </c>
+      <c r="F13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Research</v>
+      </c>
+      <c r="G13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>Rare Diseases</v>
+      </c>
+      <c r="H13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Trials and Supportive Activities</v>
+      </c>
+      <c r="I13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>Genetics</v>
       </c>
-      <c r="E13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
-        <v>Clinical Research</v>
-      </c>
-      <c r="F13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+        <v>Genetics</v>
+      </c>
+      <c r="K13" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
+        <v>Genetics</v>
+      </c>
+      <c r="L13" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B13, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
-      <c r="G13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
-        <v>Genetics</v>
-      </c>
-      <c r="H13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
-        <v>Genetics</v>
-      </c>
-      <c r="I13" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
-        <v>Genetics</v>
-      </c>
-      <c r="J13" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B13, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
-        <v>Rare Diseases</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>34</v>
       </c>
@@ -1375,39 +1497,47 @@
         <v>35</v>
       </c>
       <c r="C14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>Clinical Research</v>
       </c>
       <c r="D14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <v>Genetics</v>
+      </c>
+      <c r="E14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>Clinical Trials and Supportive Activities</v>
+      </c>
+      <c r="F14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <v>Genetics</v>
+      </c>
+      <c r="G14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>Clinical Research</v>
       </c>
-      <c r="E14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
-        <v>Genetics</v>
-      </c>
-      <c r="F14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
-        <v>Clinical Research</v>
-      </c>
-      <c r="G14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
-      <c r="H14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="I14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>Rare Diseases</v>
+      </c>
+      <c r="J14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
-      <c r="I14" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K14" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>Prevention</v>
       </c>
-      <c r="J14" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B14, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L14" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B14, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>36</v>
       </c>
@@ -1415,112 +1545,136 @@
         <v>37</v>
       </c>
       <c r="C15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
       <c r="D15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
       <c r="E15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>Patient Safety</v>
+      </c>
+      <c r="F15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
-      <c r="F15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
-      <c r="G15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>Hematology</v>
+      </c>
+      <c r="I15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>Biotechnology</v>
       </c>
-      <c r="H15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>Rare Diseases</v>
       </c>
-      <c r="I15" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K15" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>Clinical Research</v>
       </c>
-      <c r="J15" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B15, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L15" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B15, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>Digestive Diseases</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="C16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="D16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="E16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="F16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="G16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="H16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="I16" s="6" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
-      <c r="J16" s="8" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B16, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J16" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="6" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
+        <v/>
+      </c>
+      <c r="L16" s="8" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B16, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="str">
         <f>"- - FOR RESEARCHERS FUNDED BY AGENCY: - -"</f>
         <v>- - FOR RESEARCHERS FUNDED BY AGENCY: - -</v>
       </c>
       <c r="C17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="D17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="E17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="F17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="G17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="H17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
       <c r="I17" s="15" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
-      <c r="J17" s="16" t="str">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B17, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J17" s="15" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="15" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
+        <v/>
+      </c>
+      <c r="L17" s="16" t="str">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B17, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>38</v>
       </c>
@@ -1528,39 +1682,47 @@
         <v>39</v>
       </c>
       <c r="C18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0.47619047619047622</v>
       </c>
       <c r="D18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0.56451612903225812</v>
       </c>
       <c r="E18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.66739606126914663</v>
+      </c>
+      <c r="F18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.61940298507462688</v>
       </c>
-      <c r="F18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="G18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.46153846153846162</v>
+      </c>
+      <c r="I18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>2.2982300884955751</v>
       </c>
-      <c r="H18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1.572225619076735</v>
       </c>
-      <c r="I18" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K18" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1.7541782729805011</v>
       </c>
-      <c r="J18" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B18, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L18" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B18, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1.846341463414634</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>40</v>
       </c>
@@ -1568,119 +1730,143 @@
         <v>41</v>
       </c>
       <c r="C19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="H19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J19" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="I19" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K19" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="J19" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B19, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L19" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B19, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>221448.99642857141</v>
       </c>
-      <c r="D20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+      <c r="D20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>272224.1048387097</v>
       </c>
-      <c r="E20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+      <c r="E20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>328297.89059080958</v>
+      </c>
+      <c r="F20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>275667.85074626858</v>
       </c>
-      <c r="F20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>231083.48571428569</v>
       </c>
-      <c r="G20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>147999.29230769229</v>
+      </c>
+      <c r="I20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>995631.25575221237</v>
       </c>
-      <c r="H20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1850934.36953531</v>
       </c>
-      <c r="I20" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K20" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1248767.869428969</v>
       </c>
-      <c r="J20" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B20, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L20" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B20, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>2457502.4487804882</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="9" t="s">
         <v>44</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="G21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>170122</v>
       </c>
-      <c r="I21" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K21" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>344062.5</v>
       </c>
-      <c r="J21" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B21, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L21" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B21, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>46</v>
       </c>
@@ -1688,39 +1874,47 @@
         <v>47</v>
       </c>
       <c r="C22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
-        <v>0.34417917328139719</v>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.34417917328139741</v>
       </c>
       <c r="D22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0.37335698640743747</v>
       </c>
       <c r="E22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.43745432719414279</v>
+      </c>
+      <c r="F22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.4388717372043891</v>
       </c>
-      <c r="F22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>0.19048793215916501</v>
       </c>
-      <c r="G22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.39742887249736569</v>
+      </c>
+      <c r="I22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.99660313009777179</v>
       </c>
-      <c r="H22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.8720131732351345</v>
       </c>
-      <c r="I22" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K22" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>0.67260028619854684</v>
       </c>
-      <c r="J22" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B22, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L22" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B22, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.76940160555902304</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>48</v>
       </c>
@@ -1728,39 +1922,47 @@
         <v>49</v>
       </c>
       <c r="C23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.8850726442507264</v>
       </c>
-      <c r="H23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J23" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="I23" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K23" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>0.50068493150684934</v>
       </c>
-      <c r="J23" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B23, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L23" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B23, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.15582191780821919</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>50</v>
       </c>
@@ -1768,39 +1970,47 @@
         <v>51</v>
       </c>
       <c r="C24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0.22626133786848079</v>
       </c>
       <c r="D24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0.2043970814132105</v>
       </c>
       <c r="E24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.2476902504254801</v>
+      </c>
+      <c r="F24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.33843283582089562</v>
       </c>
-      <c r="F24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>0.13714285714285709</v>
       </c>
-      <c r="G24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.2153846153846154</v>
+      </c>
+      <c r="I24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.54649152420280922</v>
       </c>
-      <c r="H24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.31853114978013802</v>
       </c>
-      <c r="I24" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K24" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1.0497777742591501</v>
       </c>
-      <c r="J24" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B24, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L24" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B24, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.75571702267798491</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>52</v>
       </c>
@@ -1808,39 +2018,47 @@
         <v>53</v>
       </c>
       <c r="C25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="H25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J25" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.2</v>
       </c>
-      <c r="I25" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K25" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>0.6</v>
       </c>
-      <c r="J25" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B25, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L25" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B25, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>54</v>
       </c>
@@ -1848,39 +2066,47 @@
         <v>55</v>
       </c>
       <c r="C26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>38.268357810413882</v>
       </c>
       <c r="D26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>28.413793103448281</v>
       </c>
       <c r="E26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>53.682222222222222</v>
+      </c>
+      <c r="F26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>36.85820895522388</v>
       </c>
-      <c r="F26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>22.714285714285719</v>
       </c>
-      <c r="G26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>41.430769230769229</v>
+      </c>
+      <c r="I26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>29.878932968536251</v>
       </c>
-      <c r="H26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>29.544078767435501</v>
       </c>
-      <c r="I26" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K26" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>28.548582054858201</v>
       </c>
-      <c r="J26" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B26, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L26" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B26, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>21.42244224422442</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>56</v>
       </c>
@@ -1888,39 +2114,47 @@
         <v>57</v>
       </c>
       <c r="C27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>23</v>
       </c>
       <c r="D27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>18.5</v>
       </c>
       <c r="E27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>44</v>
+      </c>
+      <c r="F27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>25</v>
       </c>
-      <c r="F27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>19</v>
       </c>
-      <c r="G27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>38</v>
+      </c>
+      <c r="I27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>21</v>
       </c>
-      <c r="H27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>19</v>
       </c>
-      <c r="I27" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K27" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>19</v>
       </c>
-      <c r="J27" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B27, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L27" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B27, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>58</v>
       </c>
@@ -1928,39 +2162,47 @@
         <v>59</v>
       </c>
       <c r="C28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>1610.30173564753</v>
       </c>
       <c r="D28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>794.89655172413791</v>
       </c>
       <c r="E28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>1943.935555555556</v>
+      </c>
+      <c r="F28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>2513.656716417911</v>
       </c>
-      <c r="F28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>518.2285714285714</v>
       </c>
-      <c r="G28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>1625.9846153846149</v>
+      </c>
+      <c r="I28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>2095.6251709986318</v>
       </c>
-      <c r="H28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1895.7867626948671</v>
       </c>
-      <c r="I28" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K28" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1660.812180381218</v>
       </c>
-      <c r="J28" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B28, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L28" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B28, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1573.3531353135311</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>60</v>
       </c>
@@ -1968,39 +2210,47 @@
         <v>61</v>
       </c>
       <c r="C29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>762</v>
       </c>
       <c r="D29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>350</v>
       </c>
       <c r="E29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>1125</v>
+      </c>
+      <c r="F29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>839.5</v>
       </c>
-      <c r="F29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>291</v>
       </c>
-      <c r="G29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>1006</v>
+      </c>
+      <c r="I29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1080.5</v>
       </c>
-      <c r="H29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>911</v>
       </c>
-      <c r="I29" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K29" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>897</v>
       </c>
-      <c r="J29" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B29, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L29" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B29, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>525</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>62</v>
       </c>
@@ -2008,39 +2258,47 @@
         <v>63</v>
       </c>
       <c r="C30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0.64880952380952384</v>
       </c>
       <c r="D30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0.20161290322580641</v>
       </c>
       <c r="E30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.7286652078774617</v>
+      </c>
+      <c r="F30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.82089552238805974</v>
       </c>
-      <c r="F30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>0.1714285714285714</v>
       </c>
-      <c r="G30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="I30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>2.385840707964602</v>
       </c>
-      <c r="H30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1.6859523081626411</v>
       </c>
-      <c r="I30" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K30" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1.991991643454039</v>
       </c>
-      <c r="J30" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B30, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L30" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B30, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1.9829268292682929</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>64</v>
       </c>
@@ -2048,119 +2306,143 @@
         <v>65</v>
       </c>
       <c r="C31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="H31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J31" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="I31" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K31" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="J31" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B31, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L31" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B31, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>66</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>472682.62023809517</v>
       </c>
-      <c r="D32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+      <c r="D32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>263220.22580645158</v>
       </c>
-      <c r="E32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+      <c r="E32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>475689.35010940919</v>
+      </c>
+      <c r="F32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>729368.1268656716</v>
       </c>
-      <c r="F32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>66027.942857142858</v>
       </c>
-      <c r="G32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>539939.73846153845</v>
+      </c>
+      <c r="I32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1622308.2743362831</v>
       </c>
-      <c r="H32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>2466313.82115561</v>
       </c>
-      <c r="I32" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K32" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1948413.328690808</v>
       </c>
-      <c r="J32" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B32, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L32" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B32, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>3485941.704878049</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>68</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="D33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="E33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="F33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="C33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="D33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="E33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>344460</v>
       </c>
-      <c r="I33" s="21">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K33" s="22">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>678402</v>
       </c>
-      <c r="J33" s="22">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B33, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L33" s="23">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B33, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>24213</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>70</v>
       </c>
@@ -2168,39 +2450,47 @@
         <v>71</v>
       </c>
       <c r="C34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
-        <v>0.50165428279951729</v>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.50165428279951751</v>
       </c>
       <c r="D34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0.1977117506987203</v>
       </c>
       <c r="E34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.55719659825202239</v>
+      </c>
+      <c r="F34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.68997580590199692</v>
       </c>
-      <c r="F34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>0.1708962818003914</v>
       </c>
-      <c r="G34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.63188268352651911</v>
+      </c>
+      <c r="I34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.9625873149534101</v>
       </c>
-      <c r="H34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.94556933530859999</v>
       </c>
-      <c r="I34" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K34" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>0.8477949844168664</v>
       </c>
-      <c r="J34" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B34, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L34" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B34, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.84745213061594205</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>72</v>
       </c>
@@ -2208,39 +2498,47 @@
         <v>73</v>
       </c>
       <c r="C35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I35" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="H35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J35" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.50091324200913245</v>
       </c>
-      <c r="I35" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K35" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>0.81867995018679951</v>
       </c>
-      <c r="J35" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B35, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L35" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B35, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.50058708414872799</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>74</v>
       </c>
@@ -2248,39 +2546,47 @@
         <v>75</v>
       </c>
       <c r="C36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0.30877267573696149</v>
       </c>
       <c r="D36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>9.0572196620583717E-2</v>
       </c>
       <c r="E36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.2903355215171407</v>
+      </c>
+      <c r="F36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0.34141791044776121</v>
       </c>
-      <c r="F36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>7.2380952380952379E-2</v>
       </c>
-      <c r="G36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0.33076923076923082</v>
+      </c>
+      <c r="I36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.64156601211524689</v>
       </c>
-      <c r="H36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.43033097410144833</v>
       </c>
-      <c r="I36" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K36" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1.3895763372013741</v>
       </c>
-      <c r="J36" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B36, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L36" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B36, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.95609296745088013</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>76</v>
       </c>
@@ -2288,39 +2594,47 @@
         <v>77</v>
       </c>
       <c r="C37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="D37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="E37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="F37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>0</v>
       </c>
       <c r="G37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>0.375</v>
       </c>
-      <c r="H37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J37" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>0.2857142857142857</v>
       </c>
-      <c r="I37" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K37" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1</v>
       </c>
-      <c r="J37" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B37, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L37" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B37, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>78</v>
       </c>
@@ -2328,39 +2642,47 @@
         <v>79</v>
       </c>
       <c r="C38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>49.778371161548733</v>
       </c>
       <c r="D38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>41.793103448275858</v>
       </c>
       <c r="E38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>73.731111111111105</v>
+      </c>
+      <c r="F38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>50.828358208955223</v>
       </c>
-      <c r="F38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>30.542857142857141</v>
       </c>
-      <c r="G38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>56.153846153846153</v>
+      </c>
+      <c r="I38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>39.755813953488371</v>
       </c>
-      <c r="H38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>40.244142583644823</v>
       </c>
-      <c r="I38" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K38" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>43.242212924221292</v>
       </c>
-      <c r="J38" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B38, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L38" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B38, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>28.57755775577558</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>80</v>
       </c>
@@ -2368,39 +2690,47 @@
         <v>81</v>
       </c>
       <c r="C39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>31</v>
       </c>
       <c r="D39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>22.5</v>
       </c>
       <c r="E39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>61</v>
+      </c>
+      <c r="F39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>37</v>
       </c>
-      <c r="F39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>20</v>
       </c>
-      <c r="G39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>45</v>
+      </c>
+      <c r="I39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>29</v>
       </c>
-      <c r="H39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>27</v>
       </c>
-      <c r="I39" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K39" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>30</v>
       </c>
-      <c r="J39" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B39, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L39" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B39, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>82</v>
       </c>
@@ -2408,39 +2738,47 @@
         <v>83</v>
       </c>
       <c r="C40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>1243.2643524699599</v>
       </c>
       <c r="D40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>564.68103448275861</v>
       </c>
       <c r="E40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>1481.18</v>
+      </c>
+      <c r="F40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>1971.268656716418</v>
       </c>
-      <c r="F40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>258.54285714285709</v>
       </c>
-      <c r="G40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>1258.184615384615</v>
+      </c>
+      <c r="I40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>1662.4247606019151</v>
       </c>
-      <c r="H40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>1485.413620202389</v>
       </c>
-      <c r="I40" s="12">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K40" s="12">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>1553.2152487215251</v>
       </c>
-      <c r="J40" s="13">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B40, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L40" s="13">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B40, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>1508.280528052805</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>84</v>
       </c>
@@ -2448,35 +2786,43 @@
         <v>85</v>
       </c>
       <c r="C41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(C$2, RAW!$1:$1, 0)), "")</f>
         <v>568</v>
       </c>
       <c r="D41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(D$2, RAW!$1:$1, 0)), "")</f>
         <v>181</v>
       </c>
       <c r="E41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(E$2, RAW!$1:$1, 0)), "")</f>
+        <v>879</v>
+      </c>
+      <c r="F41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
         <v>630</v>
       </c>
-      <c r="F41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(F$2, RAW!$1:$1, 0)), "")</f>
+      <c r="G41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
         <v>190</v>
       </c>
-      <c r="G41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(G$2, RAW!$1:$1, 0)), "")</f>
+      <c r="H41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+        <v>786</v>
+      </c>
+      <c r="I41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
         <v>835</v>
       </c>
-      <c r="H41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(H$2, RAW!$1:$1, 0)), "")</f>
+      <c r="J41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
         <v>640</v>
       </c>
-      <c r="I41" s="19">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(I$2, RAW!$1:$1, 0)), "")</f>
+      <c r="K41" s="19">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(K$2, RAW!$1:$1, 0)), "")</f>
         <v>765</v>
       </c>
-      <c r="J41" s="20">
-        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$I$38, MATCH($B41, RAW!$A:$A, 0), MATCH(J$2, RAW!$1:$1, 0)), "")</f>
+      <c r="L41" s="20">
+        <f>_xlfn.IFNA(INDEX(RAW!$A$1:$K$38, MATCH($B41, RAW!$A:$A, 0), MATCH(L$2, RAW!$1:$1, 0)), "")</f>
         <v>400</v>
       </c>
     </row>
@@ -2488,43 +2834,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="23" t="s">
+      <c r="B1" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="F1" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="J1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="K1" s="24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>17</v>
       </c>
       <c r="C2">
@@ -2540,17 +2892,23 @@
         <v>464458.65151515149</v>
       </c>
       <c r="G2">
+        <v>442562.60098522168</v>
+      </c>
+      <c r="H2">
+        <v>420509.171875</v>
+      </c>
+      <c r="I2">
         <v>1856361.57394931</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>609689.00565504236</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>797713.74712643679</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
         <v>19</v>
       </c>
       <c r="C3">
@@ -2566,17 +2924,23 @@
         <v>471555</v>
       </c>
       <c r="G3">
+        <v>390888.5</v>
+      </c>
+      <c r="H3">
+        <v>363145</v>
+      </c>
+      <c r="I3">
         <v>732061</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>433722</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>325304</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="24" t="s">
         <v>21</v>
       </c>
       <c r="B4">
@@ -2595,17 +2959,23 @@
         <v>2.6584059775840601</v>
       </c>
       <c r="G4">
+        <v>3.194426074633903</v>
+      </c>
+      <c r="H4">
+        <v>3.114340753424655</v>
+      </c>
+      <c r="I4">
         <v>4.2549639405647506</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>2.8267044860399211</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>3.2201228153046779</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="24" t="s">
         <v>23</v>
       </c>
       <c r="B5">
@@ -2624,17 +2994,23 @@
         <v>3</v>
       </c>
       <c r="G5">
+        <v>3.0027397260273969</v>
+      </c>
+      <c r="H5">
+        <v>3.0027397260273969</v>
+      </c>
+      <c r="I5">
         <v>3.9589041095890409</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>3</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>3.0849315068493151</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="24" t="s">
         <v>25</v>
       </c>
       <c r="B6">
@@ -2653,17 +3029,23 @@
         <v>1.492424242424242</v>
       </c>
       <c r="G6">
+        <v>1.157635467980296</v>
+      </c>
+      <c r="H6">
+        <v>1.234375</v>
+      </c>
+      <c r="I6">
         <v>1.104041853008185</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>2.6992481203007519</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>1.57088122605364</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
         <v>27</v>
       </c>
       <c r="B7">
@@ -2685,14 +3067,20 @@
         <v>1</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
         <v>13</v>
       </c>
       <c r="B8">
@@ -2711,17 +3099,23 @@
         <v>132</v>
       </c>
       <c r="G8">
+        <v>406</v>
+      </c>
+      <c r="H8">
+        <v>64</v>
+      </c>
+      <c r="I8">
         <v>12468</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>1064</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>261</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="24" t="s">
         <v>15</v>
       </c>
       <c r="B9">
@@ -2740,17 +3134,23 @@
         <v>95</v>
       </c>
       <c r="G9">
+        <v>333</v>
+      </c>
+      <c r="H9">
+        <v>50</v>
+      </c>
+      <c r="I9">
         <v>8450</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>1944</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>328</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="23" t="s">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="24" t="s">
         <v>71</v>
       </c>
       <c r="B10">
@@ -2763,23 +3163,29 @@
         <v>0.1708962818003914</v>
       </c>
       <c r="E10">
-        <v>0.50165428279951729</v>
+        <v>0.50165428279951751</v>
       </c>
       <c r="F10">
         <v>0.68997580590199692</v>
       </c>
       <c r="G10">
+        <v>0.55719659825202239</v>
+      </c>
+      <c r="H10">
+        <v>0.63188268352651911</v>
+      </c>
+      <c r="I10">
         <v>0.94556933530859999</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.8477949844168664</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>0.84745213061594205</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="23" t="s">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="24" t="s">
         <v>73</v>
       </c>
       <c r="B11">
@@ -2798,17 +3204,23 @@
         <v>0</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>0.50091324200913245</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>0.81867995018679951</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>0.50058708414872799</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="23" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="24" t="s">
         <v>75</v>
       </c>
       <c r="B12">
@@ -2827,17 +3239,23 @@
         <v>0.34141791044776121</v>
       </c>
       <c r="G12">
+        <v>0.2903355215171407</v>
+      </c>
+      <c r="H12">
+        <v>0.33076923076923082</v>
+      </c>
+      <c r="I12">
         <v>0.43033097410144833</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>1.3895763372013741</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>0.95609296745088013</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="24" t="s">
         <v>77</v>
       </c>
       <c r="B13">
@@ -2856,17 +3274,23 @@
         <v>0</v>
       </c>
       <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
         <v>0.2857142857142857</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>1</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="23" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="24" t="s">
         <v>83</v>
       </c>
       <c r="B14">
@@ -2885,17 +3309,23 @@
         <v>1971.268656716418</v>
       </c>
       <c r="G14">
+        <v>1481.18</v>
+      </c>
+      <c r="H14">
+        <v>1258.184615384615</v>
+      </c>
+      <c r="I14">
         <v>1485.413620202389</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>1553.2152487215251</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>1508.280528052805</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="23" t="s">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="24" t="s">
         <v>85</v>
       </c>
       <c r="B15">
@@ -2914,17 +3344,23 @@
         <v>630</v>
       </c>
       <c r="G15">
+        <v>879</v>
+      </c>
+      <c r="H15">
+        <v>786</v>
+      </c>
+      <c r="I15">
         <v>640</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>765</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>400</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="23" t="s">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="24" t="s">
         <v>67</v>
       </c>
       <c r="B16">
@@ -2943,17 +3379,23 @@
         <v>729368.1268656716</v>
       </c>
       <c r="G16">
+        <v>475689.35010940919</v>
+      </c>
+      <c r="H16">
+        <v>539939.73846153845</v>
+      </c>
+      <c r="I16">
         <v>2466313.82115561</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>1948413.328690808</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>3485941.704878049</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="24" t="s">
         <v>69</v>
       </c>
       <c r="B17">
@@ -2972,17 +3414,23 @@
         <v>0</v>
       </c>
       <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
         <v>344460</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>678402</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>24213</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="23" t="s">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="24" t="s">
         <v>63</v>
       </c>
       <c r="B18">
@@ -3001,17 +3449,23 @@
         <v>0.82089552238805974</v>
       </c>
       <c r="G18">
+        <v>0.7286652078774617</v>
+      </c>
+      <c r="H18">
+        <v>0.69230769230769229</v>
+      </c>
+      <c r="I18">
         <v>1.6859523081626411</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>1.991991643454039</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>1.9829268292682929</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="23" t="s">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
         <v>65</v>
       </c>
       <c r="B19">
@@ -3030,17 +3484,23 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="23" t="s">
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="24" t="s">
         <v>79</v>
       </c>
       <c r="B20">
@@ -3059,17 +3519,23 @@
         <v>50.828358208955223</v>
       </c>
       <c r="G20">
+        <v>73.731111111111105</v>
+      </c>
+      <c r="H20">
+        <v>56.153846153846153</v>
+      </c>
+      <c r="I20">
         <v>40.244142583644823</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>43.242212924221292</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>28.57755775577558</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="23" t="s">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
         <v>81</v>
       </c>
       <c r="B21">
@@ -3088,17 +3554,23 @@
         <v>37</v>
       </c>
       <c r="G21">
+        <v>61</v>
+      </c>
+      <c r="H21">
+        <v>45</v>
+      </c>
+      <c r="I21">
         <v>27</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>30</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="24" t="s">
         <v>47</v>
       </c>
       <c r="B22">
@@ -3111,23 +3583,29 @@
         <v>0.19048793215916501</v>
       </c>
       <c r="E22">
-        <v>0.34417917328139719</v>
+        <v>0.34417917328139741</v>
       </c>
       <c r="F22">
         <v>0.4388717372043891</v>
       </c>
       <c r="G22">
+        <v>0.43745432719414279</v>
+      </c>
+      <c r="H22">
+        <v>0.39742887249736569</v>
+      </c>
+      <c r="I22">
         <v>0.8720131732351345</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>0.67260028619854684</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>0.76940160555902304</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="24" t="s">
         <v>49</v>
       </c>
       <c r="B23">
@@ -3146,17 +3624,23 @@
         <v>0</v>
       </c>
       <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
         <v>0.33333333333333331</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>0.50068493150684934</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>0.15582191780821919</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="24" t="s">
         <v>51</v>
       </c>
       <c r="B24">
@@ -3175,17 +3659,23 @@
         <v>0.33843283582089562</v>
       </c>
       <c r="G24">
+        <v>0.2476902504254801</v>
+      </c>
+      <c r="H24">
+        <v>0.2153846153846154</v>
+      </c>
+      <c r="I24">
         <v>0.31853114978013802</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>1.0497777742591501</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>0.75571702267798491</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
       <c r="B25">
@@ -3204,17 +3694,23 @@
         <v>0</v>
       </c>
       <c r="G25">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
+      <c r="J25">
+        <v>0.6</v>
+      </c>
+      <c r="K25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="24" t="s">
         <v>59</v>
       </c>
       <c r="B26">
@@ -3233,17 +3729,23 @@
         <v>2513.656716417911</v>
       </c>
       <c r="G26">
+        <v>1943.935555555556</v>
+      </c>
+      <c r="H26">
+        <v>1625.9846153846149</v>
+      </c>
+      <c r="I26">
         <v>1895.7867626948671</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>1660.812180381218</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>1573.3531353135311</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="23" t="s">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="24" t="s">
         <v>61</v>
       </c>
       <c r="B27">
@@ -3262,17 +3764,23 @@
         <v>839.5</v>
       </c>
       <c r="G27">
+        <v>1125</v>
+      </c>
+      <c r="H27">
+        <v>1006</v>
+      </c>
+      <c r="I27">
         <v>911</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>897</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="23" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="24" t="s">
         <v>43</v>
       </c>
       <c r="B28">
@@ -3291,17 +3799,23 @@
         <v>275667.85074626858</v>
       </c>
       <c r="G28">
+        <v>328297.89059080958</v>
+      </c>
+      <c r="H28">
+        <v>147999.29230769229</v>
+      </c>
+      <c r="I28">
         <v>1850934.36953531</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>1248767.869428969</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>2457502.4487804882</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="23" t="s">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="24" t="s">
         <v>45</v>
       </c>
       <c r="B29">
@@ -3320,17 +3834,23 @@
         <v>0</v>
       </c>
       <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29">
         <v>170122</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>344062.5</v>
       </c>
-      <c r="I29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="K29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="24" t="s">
         <v>39</v>
       </c>
       <c r="B30">
@@ -3349,17 +3869,23 @@
         <v>0.61940298507462688</v>
       </c>
       <c r="G30">
+        <v>0.66739606126914663</v>
+      </c>
+      <c r="H30">
+        <v>0.46153846153846162</v>
+      </c>
+      <c r="I30">
         <v>1.572225619076735</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>1.7541782729805011</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>1.846341463414634</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="23" t="s">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="24" t="s">
         <v>41</v>
       </c>
       <c r="B31">
@@ -3378,17 +3904,23 @@
         <v>0</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="23" t="s">
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="24" t="s">
         <v>55</v>
       </c>
       <c r="B32">
@@ -3407,17 +3939,23 @@
         <v>36.85820895522388</v>
       </c>
       <c r="G32">
+        <v>53.682222222222222</v>
+      </c>
+      <c r="H32">
+        <v>41.430769230769229</v>
+      </c>
+      <c r="I32">
         <v>29.544078767435501</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>28.548582054858201</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>21.42244224422442</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="23" t="s">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="24" t="s">
         <v>57</v>
       </c>
       <c r="B33">
@@ -3436,158 +3974,194 @@
         <v>25</v>
       </c>
       <c r="G33">
+        <v>44</v>
+      </c>
+      <c r="H33">
+        <v>38</v>
+      </c>
+      <c r="I33">
         <v>19</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>19</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="23" t="s">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="24" t="s">
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H34" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="I34" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="J34" t="s">
+        <v>88</v>
+      </c>
+      <c r="K34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="24" t="s">
         <v>31</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D35" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" t="s">
+        <v>90</v>
+      </c>
+      <c r="F35" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" t="s">
         <v>89</v>
       </c>
-      <c r="E35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F35" t="s">
-        <v>88</v>
-      </c>
-      <c r="G35" t="s">
-        <v>87</v>
-      </c>
       <c r="H35" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="I35" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="23" t="s">
+      <c r="J35" t="s">
+        <v>90</v>
+      </c>
+      <c r="K35" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="24" t="s">
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C36" t="s">
         <v>89</v>
       </c>
       <c r="D36" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" t="s">
         <v>89</v>
       </c>
-      <c r="F36" t="s">
-        <v>87</v>
-      </c>
       <c r="G36" t="s">
+        <v>90</v>
+      </c>
+      <c r="H36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>90</v>
+      </c>
+      <c r="C37" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" t="s">
         <v>89</v>
       </c>
-      <c r="H36" t="s">
+      <c r="E37" t="s">
         <v>89</v>
       </c>
-      <c r="I36" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>88</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
-      </c>
-      <c r="E37" t="s">
-        <v>87</v>
-      </c>
       <c r="F37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G37" t="s">
+        <v>92</v>
+      </c>
+      <c r="H37" t="s">
+        <v>90</v>
+      </c>
+      <c r="I37" t="s">
+        <v>93</v>
+      </c>
+      <c r="J37" t="s">
+        <v>94</v>
+      </c>
+      <c r="K37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>93</v>
+      </c>
+      <c r="E38" t="s">
+        <v>93</v>
+      </c>
+      <c r="F38" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" t="s">
+        <v>95</v>
+      </c>
+      <c r="H38" t="s">
+        <v>96</v>
+      </c>
+      <c r="I38" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" t="s">
         <v>89</v>
       </c>
-      <c r="G37" t="s">
-        <v>90</v>
-      </c>
-      <c r="H37" t="s">
-        <v>91</v>
-      </c>
-      <c r="I37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>90</v>
-      </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
-      <c r="D38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" t="s">
-        <v>90</v>
-      </c>
-      <c r="G38" t="s">
-        <v>88</v>
-      </c>
-      <c r="H38" t="s">
-        <v>87</v>
-      </c>
-      <c r="I38" t="s">
-        <v>92</v>
+      <c r="K38" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>